<commit_message>
App closes after finished.
</commit_message>
<xml_diff>
--- a/Server Space Analyzer/bin/Debug/Server Spaces.xlsx
+++ b/Server Space Analyzer/bin/Debug/Server Spaces.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="317">
   <si>
     <t/>
   </si>
@@ -38,19 +38,19 @@
     <t>465.54 GB</t>
   </si>
   <si>
-    <t>444.42 GB</t>
+    <t>443.69 GB</t>
   </si>
   <si>
     <t>KM-MSP</t>
   </si>
   <si>
-    <t>443.2 GB</t>
+    <t>442.84 GB</t>
   </si>
   <si>
     <t>PE-MSP</t>
   </si>
   <si>
-    <t>439.38 GB</t>
+    <t>439.39 GB</t>
   </si>
   <si>
     <t>PM-MSP</t>
@@ -59,7 +59,7 @@
     <t>465.55 GB</t>
   </si>
   <si>
-    <t>445.54 GB</t>
+    <t>444.22 GB</t>
   </si>
   <si>
     <t>RG-MSP</t>
@@ -68,7 +68,7 @@
     <t>231.9 GB</t>
   </si>
   <si>
-    <t>205.45 GB</t>
+    <t>205.33 GB</t>
   </si>
   <si>
     <t>System Reserved (D:)</t>
@@ -83,13 +83,13 @@
     <t>SE-MSP</t>
   </si>
   <si>
-    <t>440.37 GB</t>
+    <t>439.72 GB</t>
   </si>
   <si>
     <t>VE-MSP</t>
   </si>
   <si>
-    <t>439.56 GB</t>
+    <t>440.14 GB</t>
   </si>
   <si>
     <t>NKRC</t>
@@ -98,7 +98,7 @@
     <t>146.39 GB</t>
   </si>
   <si>
-    <t>31.01 GB</t>
+    <t>30.67 GB</t>
   </si>
   <si>
     <t>Back1 (D:)</t>
@@ -107,7 +107,7 @@
     <t>2794.52 GB</t>
   </si>
   <si>
-    <t>1587.94 GB</t>
+    <t>1578.47 GB</t>
   </si>
   <si>
     <t>Data (E:)</t>
@@ -116,7 +116,7 @@
     <t>488.28 GB</t>
   </si>
   <si>
-    <t>457.6 GB</t>
+    <t>457.59 GB</t>
   </si>
   <si>
     <t>RCFP (F:)</t>
@@ -125,7 +125,7 @@
     <t>390.62 GB</t>
   </si>
   <si>
-    <t>265.89 GB</t>
+    <t>265.92 GB</t>
   </si>
   <si>
     <t>RCManage_Data (G:)</t>
@@ -134,7 +134,7 @@
     <t>146.48 GB</t>
   </si>
   <si>
-    <t>1.37 GB</t>
+    <t>1.36 GB</t>
   </si>
   <si>
     <t>RCDC (L:)</t>
@@ -143,7 +143,7 @@
     <t>97.66 GB</t>
   </si>
   <si>
-    <t>64.61 GB</t>
+    <t>66.62 GB</t>
   </si>
   <si>
     <t>RCFP_Data1 (N:)</t>
@@ -152,13 +152,13 @@
     <t>1953.12 GB</t>
   </si>
   <si>
-    <t>962.27 GB</t>
+    <t>959.05 GB</t>
   </si>
   <si>
     <t>RCFP_Data2 (O:)</t>
   </si>
   <si>
-    <t>592.15 GB</t>
+    <t>575.53 GB</t>
   </si>
   <si>
     <t>VMMLibrary (P:)</t>
@@ -170,13 +170,13 @@
     <t>RCManage (R:)</t>
   </si>
   <si>
-    <t>111.39 GB</t>
+    <t>111.37 GB</t>
   </si>
   <si>
     <t>NHAPPS (U:)</t>
   </si>
   <si>
-    <t>75.13 GB</t>
+    <t>75.2 GB</t>
   </si>
   <si>
     <t>PMAPPS (V:)</t>
@@ -188,7 +188,7 @@
     <t>PEAPPS (W:)</t>
   </si>
   <si>
-    <t>85.63 GB</t>
+    <t>85.6 GB</t>
   </si>
   <si>
     <t>NHAPPS</t>
@@ -200,7 +200,7 @@
     <t>126.9 GB</t>
   </si>
   <si>
-    <t>106.52 GB</t>
+    <t>106.47 GB</t>
   </si>
   <si>
     <t>Data (D:)</t>
@@ -218,7 +218,7 @@
     <t>99.98 GB</t>
   </si>
   <si>
-    <t>88.75 GB</t>
+    <t>88.74 GB</t>
   </si>
   <si>
     <t>126.99 GB</t>
@@ -233,7 +233,7 @@
     <t>39.99 GB</t>
   </si>
   <si>
-    <t>2.28 GB</t>
+    <t>1.91 GB</t>
   </si>
   <si>
     <t>80 GB</t>
@@ -245,13 +245,13 @@
     <t>RCDC</t>
   </si>
   <si>
-    <t>97.37 GB</t>
+    <t>97.25 GB</t>
   </si>
   <si>
     <t>RCFP</t>
   </si>
   <si>
-    <t>9.28 GB</t>
+    <t>8.58 GB</t>
   </si>
   <si>
     <t>RCFP_Data1 (E:)</t>
@@ -260,19 +260,19 @@
     <t>1950 GB</t>
   </si>
   <si>
-    <t>1033.44 GB</t>
+    <t>1025.44 GB</t>
   </si>
   <si>
     <t>RCFP_Data2 (F:)</t>
   </si>
   <si>
-    <t>547.81 GB</t>
+    <t>529.68 GB</t>
   </si>
   <si>
     <t>RCMANAGE</t>
   </si>
   <si>
-    <t>94.34 GB</t>
+    <t>94.24 GB</t>
   </si>
   <si>
     <t>DATA (E:)</t>
@@ -281,7 +281,7 @@
     <t>144.87 GB</t>
   </si>
   <si>
-    <t>69.68 GB</t>
+    <t>69.65 GB</t>
   </si>
   <si>
     <t>NKRN</t>
@@ -290,7 +290,7 @@
     <t>195.31 GB</t>
   </si>
   <si>
-    <t>87.06 GB</t>
+    <t>86.58 GB</t>
   </si>
   <si>
     <t>RNFP_C (F:)</t>
@@ -338,7 +338,7 @@
     <t>13033.87 GB</t>
   </si>
   <si>
-    <t>8429.63 GB</t>
+    <t>8400.26 GB</t>
   </si>
   <si>
     <t>RNDC (O:)</t>
@@ -365,7 +365,7 @@
     <t>1863.01 GB</t>
   </si>
   <si>
-    <t>10.9 GB</t>
+    <t>3.65 GB</t>
   </si>
   <si>
     <t>KHAPPS</t>
@@ -374,7 +374,7 @@
     <t>199.9 GB</t>
   </si>
   <si>
-    <t>120.17 GB</t>
+    <t>109.72 GB</t>
   </si>
   <si>
     <t>RGAPPS</t>
@@ -398,13 +398,13 @@
     <t>RNDC</t>
   </si>
   <si>
-    <t>98.94 GB</t>
+    <t>98.85 GB</t>
   </si>
   <si>
     <t>RNFP</t>
   </si>
   <si>
-    <t>50.57 GB</t>
+    <t>48.76 GB</t>
   </si>
   <si>
     <t>RNFPData1 (F:)</t>
@@ -413,13 +413,13 @@
     <t>2040 GB</t>
   </si>
   <si>
-    <t>334.26 GB</t>
+    <t>308.7 GB</t>
   </si>
   <si>
     <t>RNFPData2 (G:)</t>
   </si>
   <si>
-    <t>1433.38 GB</t>
+    <t>1406.17 GB</t>
   </si>
   <si>
     <t>RNMANAGE</t>
@@ -428,7 +428,7 @@
     <t>SYSTEM (C:)</t>
   </si>
   <si>
-    <t>91.18 GB</t>
+    <t>91.05 GB</t>
   </si>
   <si>
     <t>DATA (D:)</t>
@@ -437,7 +437,7 @@
     <t>999.87 GB</t>
   </si>
   <si>
-    <t>899.33 GB</t>
+    <t>899.3 GB</t>
   </si>
   <si>
     <t>TRAPPS</t>
@@ -452,13 +452,13 @@
     <t>334.15 GB</t>
   </si>
   <si>
-    <t>209.22 GB</t>
+    <t>209.14 GB</t>
   </si>
   <si>
     <t>10983.09 GB</t>
   </si>
   <si>
-    <t>10691.87 GB</t>
+    <t>10691.82 GB</t>
   </si>
   <si>
     <t>RSDC (F:)</t>
@@ -521,19 +521,19 @@
     <t>1862.92 GB</t>
   </si>
   <si>
-    <t>1522.98 GB</t>
+    <t>1512.94 GB</t>
   </si>
   <si>
     <t>USB-2 (Y:)</t>
   </si>
   <si>
-    <t>1067.76 GB</t>
+    <t>1059.64 GB</t>
   </si>
   <si>
     <t>DWAPPS</t>
   </si>
   <si>
-    <t>86.88 GB</t>
+    <t>86.87 GB</t>
   </si>
   <si>
     <t>Apps (D:)</t>
@@ -548,7 +548,7 @@
     <t>HPAPPS</t>
   </si>
   <si>
-    <t>19.56 GB</t>
+    <t>19.61 GB</t>
   </si>
   <si>
     <t>64.57 GB</t>
@@ -560,178 +560,187 @@
     <t>49.9 GB</t>
   </si>
   <si>
-    <t>22.9 GB</t>
+    <t>22.53 GB</t>
   </si>
   <si>
     <t>RSFP</t>
   </si>
   <si>
-    <t>13.43 GB</t>
-  </si>
-  <si>
-    <t>1330.74 GB</t>
+    <t>12.99 GB</t>
+  </si>
+  <si>
+    <t>1320.45 GB</t>
   </si>
   <si>
     <t>RSMANAGE</t>
   </si>
   <si>
+    <t>18.23 GB</t>
+  </si>
+  <si>
+    <t>906.56 GB</t>
+  </si>
+  <si>
+    <t>SEAPPS</t>
+  </si>
+  <si>
+    <t>87.07 GB</t>
+  </si>
+  <si>
+    <t>70.67 GB</t>
+  </si>
+  <si>
+    <t>VEAPPS</t>
+  </si>
+  <si>
+    <t>34.43 GB</t>
+  </si>
+  <si>
+    <t>19.06 GB</t>
+  </si>
+  <si>
+    <t>465.64 GB</t>
+  </si>
+  <si>
+    <t>424.98 GB</t>
+  </si>
+  <si>
+    <t>SLOTH</t>
+  </si>
+  <si>
+    <t>7.31 GB</t>
+  </si>
+  <si>
+    <t>Virtual_Machines (D:)</t>
+  </si>
+  <si>
+    <t>154.59 GB</t>
+  </si>
+  <si>
+    <t>42.78 GB</t>
+  </si>
+  <si>
+    <t>DO USB Backup (G:)</t>
+  </si>
+  <si>
+    <t>2794.51 GB</t>
+  </si>
+  <si>
+    <t>2376.72 GB</t>
+  </si>
+  <si>
+    <t>86.59 GB</t>
+  </si>
+  <si>
+    <t>KHTCS</t>
+  </si>
+  <si>
+    <t>930.4 GB</t>
+  </si>
+  <si>
+    <t>633.17 GB</t>
+  </si>
+  <si>
+    <t>NKHS-TCS</t>
+  </si>
+  <si>
+    <t>279.02 GB</t>
+  </si>
+  <si>
+    <t>159.87 GB</t>
+  </si>
+  <si>
+    <t>1117.33 GB</t>
+  </si>
+  <si>
+    <t>1117.13 GB</t>
+  </si>
+  <si>
+    <t>RGLAB</t>
+  </si>
+  <si>
+    <t>555.71 GB</t>
+  </si>
+  <si>
+    <t>430.85 GB</t>
+  </si>
+  <si>
+    <t>SELAB</t>
+  </si>
+  <si>
+    <t>557.65 GB</t>
+  </si>
+  <si>
+    <t>425.56 GB</t>
+  </si>
+  <si>
+    <t>ENVY</t>
+  </si>
+  <si>
+    <t>29.82 GB</t>
+  </si>
+  <si>
+    <t>2.25 GB</t>
+  </si>
+  <si>
+    <t>GREED</t>
+  </si>
+  <si>
+    <t>136.6 GB</t>
+  </si>
+  <si>
+    <t>2.3 GB</t>
+  </si>
+  <si>
+    <t>Quorum2012 (D:)</t>
+  </si>
+  <si>
+    <t>5 GB</t>
+  </si>
+  <si>
+    <t>4.92 GB</t>
+  </si>
+  <si>
+    <t>PRIDE</t>
+  </si>
+  <si>
+    <t>29.47 GB</t>
+  </si>
+  <si>
+    <t>3.92 GB</t>
+  </si>
+  <si>
+    <t>WRATH</t>
+  </si>
+  <si>
+    <t>3.9 GB</t>
+  </si>
+  <si>
+    <t>SCCMSQL</t>
+  </si>
+  <si>
+    <t>95.65 GB</t>
+  </si>
+  <si>
+    <t>29.87 GB</t>
+  </si>
+  <si>
+    <t>10.44 GB</t>
+  </si>
+  <si>
+    <t>Logs (L:)</t>
+  </si>
+  <si>
+    <t>19.87 GB</t>
+  </si>
+  <si>
     <t>18.46 GB</t>
   </si>
   <si>
-    <t>906.6 GB</t>
-  </si>
-  <si>
-    <t>SEAPPS</t>
-  </si>
-  <si>
-    <t>70.67 GB</t>
-  </si>
-  <si>
-    <t>VEAPPS</t>
-  </si>
-  <si>
-    <t>34.43 GB</t>
-  </si>
-  <si>
-    <t>19.06 GB</t>
-  </si>
-  <si>
-    <t>465.64 GB</t>
-  </si>
-  <si>
-    <t>424.98 GB</t>
-  </si>
-  <si>
-    <t>SLOTH</t>
-  </si>
-  <si>
-    <t>9.75 GB</t>
-  </si>
-  <si>
-    <t>Virtual_Machines (D:)</t>
-  </si>
-  <si>
-    <t>154.59 GB</t>
-  </si>
-  <si>
-    <t>42.78 GB</t>
-  </si>
-  <si>
-    <t>DO USB Backup (G:)</t>
-  </si>
-  <si>
-    <t>2794.51 GB</t>
-  </si>
-  <si>
-    <t>2391.6 GB</t>
-  </si>
-  <si>
-    <t>KHTCS</t>
-  </si>
-  <si>
-    <t>930.4 GB</t>
-  </si>
-  <si>
-    <t>644.15 GB</t>
-  </si>
-  <si>
-    <t>NKHS-TCS</t>
-  </si>
-  <si>
-    <t>279.02 GB</t>
-  </si>
-  <si>
-    <t>187.98 GB</t>
-  </si>
-  <si>
-    <t>1117.33 GB</t>
-  </si>
-  <si>
-    <t>1117.13 GB</t>
-  </si>
-  <si>
-    <t>RGLAB</t>
-  </si>
-  <si>
-    <t>555.71 GB</t>
-  </si>
-  <si>
-    <t>431.7 GB</t>
-  </si>
-  <si>
-    <t>SELAB</t>
-  </si>
-  <si>
-    <t>557.65 GB</t>
-  </si>
-  <si>
-    <t>426.08 GB</t>
-  </si>
-  <si>
-    <t>ENVY</t>
-  </si>
-  <si>
-    <t>29.82 GB</t>
-  </si>
-  <si>
-    <t>2.31 GB</t>
-  </si>
-  <si>
-    <t>GREED</t>
-  </si>
-  <si>
-    <t>136.6 GB</t>
-  </si>
-  <si>
-    <t>2.19 GB</t>
-  </si>
-  <si>
-    <t>Quorum2012 (D:)</t>
-  </si>
-  <si>
-    <t>5 GB</t>
-  </si>
-  <si>
-    <t>4.92 GB</t>
-  </si>
-  <si>
-    <t>PRIDE</t>
-  </si>
-  <si>
-    <t>29.47 GB</t>
-  </si>
-  <si>
-    <t>3.94 GB</t>
-  </si>
-  <si>
-    <t>WRATH</t>
-  </si>
-  <si>
-    <t>3.98 GB</t>
-  </si>
-  <si>
-    <t>SCCMSQL</t>
-  </si>
-  <si>
-    <t>95.7 GB</t>
-  </si>
-  <si>
-    <t>29.87 GB</t>
-  </si>
-  <si>
-    <t>10.43 GB</t>
-  </si>
-  <si>
-    <t>Logs (L:)</t>
-  </si>
-  <si>
-    <t>19.87 GB</t>
-  </si>
-  <si>
     <t>DODC</t>
   </si>
   <si>
-    <t>84.06 GB</t>
+    <t>83.99 GB</t>
   </si>
   <si>
     <t>DODC2</t>
@@ -740,13 +749,13 @@
     <t>74.9 GB</t>
   </si>
   <si>
-    <t>56.95 GB</t>
+    <t>56.94 GB</t>
   </si>
   <si>
     <t>DOFMP</t>
   </si>
   <si>
-    <t>72.98 GB</t>
+    <t>72.88 GB</t>
   </si>
   <si>
     <t>DOFP</t>
@@ -755,13 +764,13 @@
     <t>98.9 GB</t>
   </si>
   <si>
-    <t>46.49 GB</t>
+    <t>47.07 GB</t>
   </si>
   <si>
     <t>2000.87 GB</t>
   </si>
   <si>
-    <t>194.57 GB</t>
+    <t>191.71 GB</t>
   </si>
   <si>
     <t>DOMONITOR</t>
@@ -770,13 +779,13 @@
     <t>63.99 GB</t>
   </si>
   <si>
-    <t>46.65 GB</t>
+    <t>46.64 GB</t>
   </si>
   <si>
     <t>DORP</t>
   </si>
   <si>
-    <t>13.85 GB</t>
+    <t>13.84 GB</t>
   </si>
   <si>
     <t>Storage (E:)</t>
@@ -791,7 +800,7 @@
     <t>12 GB</t>
   </si>
   <si>
-    <t>2.04 GB</t>
+    <t>2.02 GB</t>
   </si>
   <si>
     <t>Exchange (E:)</t>
@@ -800,7 +809,7 @@
     <t>700 GB</t>
   </si>
   <si>
-    <t>163.7 GB</t>
+    <t>163.61 GB</t>
   </si>
   <si>
     <t>AV (F:)</t>
@@ -824,7 +833,7 @@
     <t>MOODLE</t>
   </si>
   <si>
-    <t>107.77 GB</t>
+    <t>107.95 GB</t>
   </si>
   <si>
     <t>NKADFS1</t>
@@ -833,25 +842,25 @@
     <t>84.9 GB</t>
   </si>
   <si>
-    <t>67.18 GB</t>
+    <t>67.07 GB</t>
   </si>
   <si>
     <t>NKADFS2</t>
   </si>
   <si>
-    <t>68.45 GB</t>
+    <t>68.37 GB</t>
   </si>
   <si>
     <t>NKADFSP1</t>
   </si>
   <si>
-    <t>58.52 GB</t>
+    <t>58.58 GB</t>
   </si>
   <si>
     <t>NKADFSP2</t>
   </si>
   <si>
-    <t>58.59 GB</t>
+    <t>58.63 GB</t>
   </si>
   <si>
     <t>NKAPPS</t>
@@ -860,7 +869,7 @@
     <t>119.9 GB</t>
   </si>
   <si>
-    <t>85.14 GB</t>
+    <t>85.06 GB</t>
   </si>
   <si>
     <t>NKCONFIG</t>
@@ -869,31 +878,31 @@
     <t>294.9 GB</t>
   </si>
   <si>
-    <t>74.59 GB</t>
+    <t>74.58 GB</t>
   </si>
   <si>
     <t>NKDIRSYNC</t>
   </si>
   <si>
-    <t>40.75 GB</t>
+    <t>40.46 GB</t>
   </si>
   <si>
     <t>NKEXCHANGE</t>
   </si>
   <si>
-    <t>65.52 GB</t>
+    <t>65.65 GB</t>
   </si>
   <si>
     <t>NKEXCHANGE2</t>
   </si>
   <si>
-    <t>101.29 GB</t>
+    <t>101.45 GB</t>
   </si>
   <si>
     <t>NKSDSMS</t>
   </si>
   <si>
-    <t>8.3 GB</t>
+    <t>8.67 GB</t>
   </si>
   <si>
     <t>Data1 (D:)</t>
@@ -914,7 +923,7 @@
     <t>NKSDWEB</t>
   </si>
   <si>
-    <t>9.39 GB</t>
+    <t>9.34 GB</t>
   </si>
   <si>
     <t>399.58 GB</t>
@@ -926,13 +935,13 @@
     <t>94.9 GB</t>
   </si>
   <si>
-    <t>54.55 GB</t>
+    <t>54.27 GB</t>
   </si>
   <si>
     <t>250 GB</t>
   </si>
   <si>
-    <t>127.03 GB</t>
+    <t>126.97 GB</t>
   </si>
   <si>
     <t>NKVMM</t>
@@ -941,7 +950,7 @@
     <t>144.66 GB</t>
   </si>
   <si>
-    <t>123.6 GB</t>
+    <t>123.55 GB</t>
   </si>
   <si>
     <t>NKVMM-Library (D:)</t>
@@ -953,7 +962,7 @@
     <t>SKYWARDDATA</t>
   </si>
   <si>
-    <t>51.74 GB</t>
+    <t>51.72 GB</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2050,7 @@
         <v>67</v>
       </c>
       <c r="D107" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108">
@@ -2053,22 +2062,22 @@
         <v>175</v>
       </c>
       <c r="D108" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="109"/>
     <row r="110">
       <c r="A110" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D110" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="111">
@@ -2077,16 +2086,16 @@
         <v>63</v>
       </c>
       <c r="C111" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D111" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="112"/>
     <row r="113">
       <c r="A113" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
@@ -2095,31 +2104,31 @@
         <v>98</v>
       </c>
       <c r="D113" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="114">
       <c r="A114"/>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C114" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D114" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115">
       <c r="A115"/>
       <c r="B115" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D115" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="116"/>
@@ -2293,7 +2302,7 @@
         <v>91</v>
       </c>
       <c r="D131" t="s">
-        <v>92</v>
+        <v>205</v>
       </c>
     </row>
     <row r="132">
@@ -2590,31 +2599,31 @@
     <row r="157"/>
     <row r="158">
       <c r="A158" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B158" t="s">
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D158" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="159"/>
     <row r="160">
       <c r="A160" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B160" t="s">
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D160" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="161">
@@ -2623,118 +2632,118 @@
         <v>32</v>
       </c>
       <c r="C161" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D161" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="162"/>
     <row r="163">
       <c r="A163" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B163" t="s">
         <v>6</v>
       </c>
       <c r="C163" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D163" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="164"/>
     <row r="165">
       <c r="A165" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B165" t="s">
         <v>6</v>
       </c>
       <c r="C165" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D165" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="166"/>
     <row r="167">
       <c r="A167" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B167" t="s">
         <v>6</v>
       </c>
       <c r="C167" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D167" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168"/>
     <row r="169">
       <c r="A169" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B169" t="s">
         <v>6</v>
       </c>
       <c r="C169" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D169" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170">
       <c r="A170"/>
       <c r="B170" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C170" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D170" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171"/>
     <row r="172">
       <c r="A172" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B172" t="s">
         <v>6</v>
       </c>
       <c r="C172" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D172" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="173"/>
     <row r="174">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D174" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="175"/>
     <row r="176">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B176" t="s">
         <v>6</v>
@@ -2743,7 +2752,7 @@
         <v>61</v>
       </c>
       <c r="D176" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="177">
@@ -2752,28 +2761,28 @@
         <v>32</v>
       </c>
       <c r="C177" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D177" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="178">
       <c r="A178"/>
       <c r="B178" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C178" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D178" t="s">
-        <v>187</v>
+        <v>240</v>
       </c>
     </row>
     <row r="179"/>
     <row r="180">
       <c r="A180" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B180" t="s">
         <v>6</v>
@@ -2782,28 +2791,28 @@
         <v>61</v>
       </c>
       <c r="D180" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="181"/>
     <row r="182">
       <c r="A182" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D182" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="183"/>
     <row r="184">
       <c r="A184" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
@@ -2812,22 +2821,22 @@
         <v>61</v>
       </c>
       <c r="D184" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185"/>
     <row r="186">
       <c r="A186" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B186" t="s">
         <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D186" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="187">
@@ -2836,31 +2845,31 @@
         <v>63</v>
       </c>
       <c r="C187" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D187" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="188"/>
     <row r="189">
       <c r="A189" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B189" t="s">
         <v>6</v>
       </c>
       <c r="C189" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D189" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="190"/>
     <row r="191">
       <c r="A191" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B191" t="s">
         <v>6</v>
@@ -2869,76 +2878,76 @@
         <v>72</v>
       </c>
       <c r="D191" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="192">
       <c r="A192"/>
       <c r="B192" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C192" t="s">
         <v>69</v>
       </c>
       <c r="D192" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="193"/>
     <row r="194">
       <c r="A194" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B194" t="s">
         <v>6</v>
       </c>
       <c r="C194" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D194" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="195">
       <c r="A195"/>
       <c r="B195" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C195" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D195" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="196">
       <c r="A196"/>
       <c r="B196" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C196" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D196" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="197">
       <c r="A197"/>
       <c r="B197" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C197" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D197" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="198"/>
     <row r="199">
       <c r="A199" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B199" t="s">
         <v>6</v>
@@ -2947,118 +2956,118 @@
         <v>69</v>
       </c>
       <c r="D199" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="200"/>
     <row r="201">
       <c r="A201" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B201" t="s">
         <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D201" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="202"/>
     <row r="203">
       <c r="A203" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
       </c>
       <c r="C203" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D203" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="204"/>
     <row r="205">
       <c r="A205" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B205" t="s">
         <v>6</v>
       </c>
       <c r="C205" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D205" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="206"/>
     <row r="207">
       <c r="A207" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B207" t="s">
         <v>6</v>
       </c>
       <c r="C207" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D207" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="208"/>
     <row r="209">
       <c r="A209" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B209" t="s">
         <v>6</v>
       </c>
       <c r="C209" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D209" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="210"/>
     <row r="211">
       <c r="A211" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B211" t="s">
         <v>6</v>
       </c>
       <c r="C211" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D211" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="212"/>
     <row r="213">
       <c r="A213" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B213" t="s">
         <v>6</v>
       </c>
       <c r="C213" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D213" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="214"/>
     <row r="215">
       <c r="A215" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B215" t="s">
         <v>6</v>
@@ -3067,13 +3076,13 @@
         <v>61</v>
       </c>
       <c r="D215" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="216"/>
     <row r="217">
       <c r="A217" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B217" t="s">
         <v>6</v>
@@ -3082,61 +3091,61 @@
         <v>61</v>
       </c>
       <c r="D217" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="218"/>
     <row r="219">
       <c r="A219" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B219" t="s">
         <v>6</v>
       </c>
       <c r="C219" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D219" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="220">
       <c r="A220"/>
       <c r="B220" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C220" t="s">
         <v>72</v>
       </c>
       <c r="D220" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="221">
       <c r="A221"/>
       <c r="B221" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C221" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D221" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="222"/>
     <row r="223">
       <c r="A223" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B223" t="s">
         <v>6</v>
       </c>
       <c r="C223" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D223" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="224">
@@ -3145,25 +3154,25 @@
         <v>63</v>
       </c>
       <c r="C224" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D224" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="225"/>
     <row r="226">
       <c r="A226" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B226" t="s">
         <v>6</v>
       </c>
       <c r="C226" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D226" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="227">
@@ -3172,43 +3181,43 @@
         <v>63</v>
       </c>
       <c r="C227" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D227" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="228"/>
     <row r="229">
       <c r="A229" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B229" t="s">
         <v>6</v>
       </c>
       <c r="C229" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D229" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="230">
       <c r="A230"/>
       <c r="B230" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C230" t="s">
         <v>88</v>
       </c>
       <c r="D230" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="231"/>
     <row r="232">
       <c r="A232" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B232" t="s">
         <v>6</v>
@@ -3217,7 +3226,7 @@
         <v>69</v>
       </c>
       <c r="D232" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added button hiding and status labels.
</commit_message>
<xml_diff>
--- a/Server Space Analyzer/bin/Debug/Server Spaces.xlsx
+++ b/Server Space Analyzer/bin/Debug/Server Spaces.xlsx
@@ -59,7 +59,7 @@
     <t>465.55 GB</t>
   </si>
   <si>
-    <t>443.86 GB</t>
+    <t>443.85 GB</t>
   </si>
   <si>
     <t>RG-MSP</t>
@@ -68,7 +68,7 @@
     <t>231.9 GB</t>
   </si>
   <si>
-    <t>204.96 GB</t>
+    <t>204.94 GB</t>
   </si>
   <si>
     <t>System Reserved (D:)</t>
@@ -98,7 +98,7 @@
     <t>146.39 GB</t>
   </si>
   <si>
-    <t>30.26 GB</t>
+    <t>30.33 GB</t>
   </si>
   <si>
     <t>Back1 (D:)</t>
@@ -176,7 +176,7 @@
     <t>NHAPPS (U:)</t>
   </si>
   <si>
-    <t>74.8 GB</t>
+    <t>75.09 GB</t>
   </si>
   <si>
     <t>PMAPPS (V:)</t>
@@ -245,13 +245,13 @@
     <t>RCDC</t>
   </si>
   <si>
-    <t>97.19 GB</t>
+    <t>97.21 GB</t>
   </si>
   <si>
     <t>RCFP</t>
   </si>
   <si>
-    <t>8.07 GB</t>
+    <t>8.13 GB</t>
   </si>
   <si>
     <t>RCFP_Data1 (E:)</t>
@@ -260,13 +260,13 @@
     <t>1950 GB</t>
   </si>
   <si>
-    <t>1021.73 GB</t>
+    <t>1021.72 GB</t>
   </si>
   <si>
     <t>RCFP_Data2 (F:)</t>
   </si>
   <si>
-    <t>527.68 GB</t>
+    <t>527.66 GB</t>
   </si>
   <si>
     <t>RCMANAGE</t>
@@ -281,7 +281,7 @@
     <t>144.87 GB</t>
   </si>
   <si>
-    <t>69.65 GB</t>
+    <t>69.63 GB</t>
   </si>
   <si>
     <t>NKRN</t>
@@ -398,7 +398,7 @@
     <t>RNDC</t>
   </si>
   <si>
-    <t>98.82 GB</t>
+    <t>98.8 GB</t>
   </si>
   <si>
     <t>RNFP</t>
@@ -413,13 +413,13 @@
     <t>2040 GB</t>
   </si>
   <si>
-    <t>301.45 GB</t>
+    <t>300.98 GB</t>
   </si>
   <si>
     <t>RNFPData2 (G:)</t>
   </si>
   <si>
-    <t>1393.91 GB</t>
+    <t>1393.48 GB</t>
   </si>
   <si>
     <t>RNMANAGE</t>
@@ -437,7 +437,7 @@
     <t>999.87 GB</t>
   </si>
   <si>
-    <t>899.3 GB</t>
+    <t>899.28 GB</t>
   </si>
   <si>
     <t>TRAPPS</t>
@@ -452,7 +452,7 @@
     <t>334.15 GB</t>
   </si>
   <si>
-    <t>209.13 GB</t>
+    <t>209.11 GB</t>
   </si>
   <si>
     <t>10983.09 GB</t>
@@ -566,7 +566,7 @@
     <t>RSFP</t>
   </si>
   <si>
-    <t>11.95 GB</t>
+    <t>11.93 GB</t>
   </si>
   <si>
     <t>1341.27 GB</t>
@@ -575,10 +575,10 @@
     <t>RSMANAGE</t>
   </si>
   <si>
-    <t>18.2 GB</t>
-  </si>
-  <si>
-    <t>906.56 GB</t>
+    <t>18.15 GB</t>
+  </si>
+  <si>
+    <t>906.54 GB</t>
   </si>
   <si>
     <t>SEAPPS</t>
@@ -608,7 +608,7 @@
     <t>SLOTH</t>
   </si>
   <si>
-    <t>9.69 GB</t>
+    <t>9.74 GB</t>
   </si>
   <si>
     <t>Virtual_Machines (D:)</t>
@@ -635,7 +635,7 @@
     <t>930.4 GB</t>
   </si>
   <si>
-    <t>631.04 GB</t>
+    <t>630.7 GB</t>
   </si>
   <si>
     <t>NKHS-TCS</t>
@@ -644,7 +644,7 @@
     <t>279.02 GB</t>
   </si>
   <si>
-    <t>153.63 GB</t>
+    <t>153.35 GB</t>
   </si>
   <si>
     <t>1117.33 GB</t>
@@ -659,7 +659,7 @@
     <t>555.71 GB</t>
   </si>
   <si>
-    <t>430.58 GB</t>
+    <t>430.92 GB</t>
   </si>
   <si>
     <t>SELAB</t>
@@ -668,7 +668,7 @@
     <t>557.65 GB</t>
   </si>
   <si>
-    <t>424.86 GB</t>
+    <t>424.88 GB</t>
   </si>
   <si>
     <t>ENVY</t>
@@ -686,7 +686,7 @@
     <t>136.6 GB</t>
   </si>
   <si>
-    <t>2.29 GB</t>
+    <t>2.28 GB</t>
   </si>
   <si>
     <t>Quorum2012 (D:)</t>
@@ -710,13 +710,13 @@
     <t>WRATH</t>
   </si>
   <si>
-    <t>3.89 GB</t>
+    <t>3.9 GB</t>
   </si>
   <si>
     <t>DODC</t>
   </si>
   <si>
-    <t>84.02 GB</t>
+    <t>84.01 GB</t>
   </si>
   <si>
     <t>DODC2</t>
@@ -725,7 +725,7 @@
     <t>74.9 GB</t>
   </si>
   <si>
-    <t>56.93 GB</t>
+    <t>56.92 GB</t>
   </si>
   <si>
     <t>DOFMP</t>
@@ -746,7 +746,7 @@
     <t>2000.87 GB</t>
   </si>
   <si>
-    <t>191.65 GB</t>
+    <t>191.64 GB</t>
   </si>
   <si>
     <t>DOMONITOR</t>
@@ -755,7 +755,7 @@
     <t>63.99 GB</t>
   </si>
   <si>
-    <t>46.65 GB</t>
+    <t>46.62 GB</t>
   </si>
   <si>
     <t>DORP</t>
@@ -785,7 +785,7 @@
     <t>700 GB</t>
   </si>
   <si>
-    <t>163.59 GB</t>
+    <t>163.58 GB</t>
   </si>
   <si>
     <t>AV (F:)</t>
@@ -824,7 +824,7 @@
     <t>NKADFS2</t>
   </si>
   <si>
-    <t>68.36 GB</t>
+    <t>68.37 GB</t>
   </si>
   <si>
     <t>NKADFSP1</t>
@@ -854,7 +854,7 @@
     <t>294.9 GB</t>
   </si>
   <si>
-    <t>74.57 GB</t>
+    <t>74.5 GB</t>
   </si>
   <si>
     <t>NKDIRSYNC</t>
@@ -917,7 +917,7 @@
     <t>250 GB</t>
   </si>
   <si>
-    <t>124.99 GB</t>
+    <t>124.97 GB</t>
   </si>
   <si>
     <t>NKVMM</t>

</xml_diff>